<commit_message>
Union DF FF Y FX funcional
</commit_message>
<xml_diff>
--- a/resources/files/OPERACIONES DE EXPORTACION 2025.xlsx
+++ b/resources/files/OPERACIONES DE EXPORTACION 2025.xlsx
@@ -1082,7 +1082,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1128,6 +1128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1233,7 +1239,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1410,36 +1416,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1453,6 +1429,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Millares 2" xfId="7"/>
@@ -2367,7 +2383,7 @@
     <col min="23" max="23" width="14.85546875" customWidth="1"/>
     <col min="24" max="24" width="21.5703125" customWidth="1"/>
     <col min="25" max="25" width="20.5703125" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="84" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" style="74" customWidth="1"/>
     <col min="27" max="27" width="19" customWidth="1"/>
     <col min="28" max="28" width="15.42578125" style="10" customWidth="1"/>
     <col min="29" max="29" width="27.28515625" customWidth="1"/>
@@ -2388,55 +2404,55 @@
   <sheetData>
     <row r="1" spans="1:16369" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="73" t="s">
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="73" t="s">
+      <c r="N1" s="82"/>
+      <c r="O1" s="82"/>
+      <c r="P1" s="82"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="76" t="s">
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="76" t="s">
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="AF1" s="78"/>
-      <c r="AG1" s="76" t="s">
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="76" t="s">
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="AJ1" s="78"/>
+      <c r="AJ1" s="76"/>
       <c r="AK1" s="18" t="s">
         <v>162</v>
       </c>
@@ -2446,14 +2462,14 @@
       <c r="AM1" s="20">
         <v>17.0626</v>
       </c>
-      <c r="AN1" s="70" t="s">
+      <c r="AN1" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="AO1" s="71"/>
-      <c r="AP1" s="71"/>
-      <c r="AQ1" s="71"/>
-      <c r="AR1" s="71"/>
-      <c r="AS1" s="72"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="79"/>
       <c r="AT1" s="7"/>
       <c r="AU1" s="7"/>
       <c r="AV1" s="7"/>
@@ -18822,7 +18838,7 @@
       <c r="N2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="86" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="29" t="s">
@@ -18855,7 +18871,7 @@
       <c r="Y2" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="32" t="s">
+      <c r="Z2" s="85" t="s">
         <v>27</v>
       </c>
       <c r="AA2" s="29" t="s">
@@ -18882,7 +18898,7 @@
       <c r="AH2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="24" t="s">
+      <c r="AI2" s="87" t="s">
         <v>31</v>
       </c>
       <c r="AJ2" s="30" t="s">
@@ -35306,7 +35322,7 @@
       <c r="Y3" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="Z3" s="80" t="s">
+      <c r="Z3" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA3" s="14">
@@ -35396,7 +35412,7 @@
       <c r="Y4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z4" s="81" t="s">
+      <c r="Z4" s="71" t="s">
         <v>298</v>
       </c>
       <c r="AA4" s="14">
@@ -35484,7 +35500,7 @@
       <c r="Y5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z5" s="81" t="s">
+      <c r="Z5" s="71" t="s">
         <v>299</v>
       </c>
       <c r="AA5" s="14">
@@ -35578,7 +35594,7 @@
       <c r="Y6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z6" s="82" t="s">
+      <c r="Z6" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA6" s="14">
@@ -35674,7 +35690,7 @@
       <c r="Y7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z7" s="82" t="s">
+      <c r="Z7" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA7" s="14">
@@ -35770,7 +35786,7 @@
       <c r="Y8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z8" s="82" t="s">
+      <c r="Z8" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA8" s="14">
@@ -35866,7 +35882,7 @@
       <c r="Y9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z9" s="82" t="s">
+      <c r="Z9" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA9" s="14">
@@ -35960,7 +35976,7 @@
       <c r="Y10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z10" s="80" t="s">
+      <c r="Z10" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA10" s="14">
@@ -36054,7 +36070,7 @@
       <c r="Y11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z11" s="80" t="s">
+      <c r="Z11" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA11" s="14">
@@ -36148,7 +36164,7 @@
       <c r="Y12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z12" s="80" t="s">
+      <c r="Z12" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA12" s="14">
@@ -36244,7 +36260,7 @@
       <c r="Y13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z13" s="80" t="s">
+      <c r="Z13" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA13" s="14">
@@ -36338,7 +36354,7 @@
       <c r="Y14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z14" s="80" t="s">
+      <c r="Z14" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA14" s="14">
@@ -36415,7 +36431,7 @@
       <c r="Y15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z15" s="80" t="s">
+      <c r="Z15" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA15" s="14">
@@ -36504,7 +36520,7 @@
       <c r="Y16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="Z16" s="82" t="s">
+      <c r="Z16" s="72" t="s">
         <v>171</v>
       </c>
       <c r="AA16" s="14">
@@ -36598,7 +36614,7 @@
       <c r="Y17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z17" s="80" t="s">
+      <c r="Z17" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA17" s="14">
@@ -36694,7 +36710,7 @@
       <c r="Y18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="82" t="s">
+      <c r="Z18" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA18" s="14">
@@ -36788,7 +36804,7 @@
       <c r="Y19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z19" s="82" t="s">
+      <c r="Z19" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA19" s="14">
@@ -36884,7 +36900,7 @@
       <c r="Y20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z20" s="82" t="s">
+      <c r="Z20" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA20" s="14">
@@ -36980,7 +36996,7 @@
       <c r="Y21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z21" s="82" t="s">
+      <c r="Z21" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA21" s="14">
@@ -37077,7 +37093,7 @@
       <c r="Y22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z22" s="82" t="s">
+      <c r="Z22" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA22" s="14">
@@ -37173,7 +37189,7 @@
       <c r="Y23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z23" s="82" t="s">
+      <c r="Z23" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA23" s="14">
@@ -37270,7 +37286,7 @@
       <c r="Y24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z24" s="82" t="s">
+      <c r="Z24" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA24" s="14">
@@ -37366,7 +37382,7 @@
       <c r="Y25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z25" s="82" t="s">
+      <c r="Z25" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA25" s="14">
@@ -37379,7 +37395,7 @@
       </c>
       <c r="AF25" s="10"/>
       <c r="AH25" s="10"/>
-      <c r="AI25">
+      <c r="AI25" s="88">
         <v>10749</v>
       </c>
       <c r="AJ25" s="42">
@@ -37462,7 +37478,7 @@
       <c r="Y26" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z26" s="82" t="s">
+      <c r="Z26" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA26" s="14">
@@ -37558,7 +37574,7 @@
       <c r="Y27" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z27" s="82" t="s">
+      <c r="Z27" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA27" s="14">
@@ -37652,7 +37668,7 @@
       <c r="Y28" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z28" s="82" t="s">
+      <c r="Z28" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA28" s="14">
@@ -37748,7 +37764,7 @@
       <c r="Y29" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z29" s="82" t="s">
+      <c r="Z29" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA29" s="14">
@@ -37844,7 +37860,7 @@
       <c r="Y30" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z30" s="82" t="s">
+      <c r="Z30" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA30" s="14">
@@ -37940,7 +37956,7 @@
       <c r="Y31" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z31" s="82" t="s">
+      <c r="Z31" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA31" s="14">
@@ -38036,7 +38052,7 @@
       <c r="Y32" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z32" s="82" t="s">
+      <c r="Z32" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA32" s="14">
@@ -38130,7 +38146,7 @@
       <c r="Y33" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="Z33" s="82" t="s">
+      <c r="Z33" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA33" s="14">
@@ -38222,7 +38238,7 @@
       <c r="Y34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Z34" s="82" t="s">
+      <c r="Z34" s="72" t="s">
         <v>171</v>
       </c>
       <c r="AA34" s="14">
@@ -38314,7 +38330,7 @@
       <c r="Y35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Z35" s="82" t="s">
+      <c r="Z35" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA35" s="14">
@@ -38388,7 +38404,7 @@
       <c r="Y36" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Z36" s="82" t="s">
+      <c r="Z36" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA36" s="14">
@@ -38464,7 +38480,7 @@
       <c r="Y37" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Z37" s="83" t="s">
+      <c r="Z37" s="73" t="s">
         <v>279</v>
       </c>
       <c r="AA37" s="14">
@@ -38533,7 +38549,7 @@
       <c r="Y38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="Z38" s="83" t="s">
+      <c r="Z38" s="73" t="s">
         <v>279</v>
       </c>
       <c r="AA38" s="14">
@@ -38622,7 +38638,7 @@
       <c r="Y39" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Z39" s="82" t="s">
+      <c r="Z39" s="72" t="s">
         <v>171</v>
       </c>
       <c r="AA39" s="14">
@@ -38710,7 +38726,7 @@
       <c r="Y40" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z40" s="82" t="s">
+      <c r="Z40" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA40" s="14">
@@ -38798,7 +38814,7 @@
       <c r="Y41" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z41" s="82" t="s">
+      <c r="Z41" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA41" s="14">
@@ -38880,7 +38896,7 @@
       <c r="Y42" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z42" s="82" t="s">
+      <c r="Z42" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA42" s="14">
@@ -38962,7 +38978,7 @@
       <c r="Y43" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z43" s="82" t="s">
+      <c r="Z43" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA43" s="14">
@@ -39044,7 +39060,7 @@
       <c r="Y44" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z44" s="82" t="s">
+      <c r="Z44" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA44" s="14">
@@ -39124,7 +39140,7 @@
       <c r="Y45" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z45" s="80" t="s">
+      <c r="Z45" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA45" s="14">
@@ -39204,7 +39220,7 @@
       <c r="Y46" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z46" s="80" t="s">
+      <c r="Z46" s="70" t="s">
         <v>277</v>
       </c>
       <c r="AA46" s="14">
@@ -39280,7 +39296,7 @@
       <c r="Y47" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Z47" s="82" t="s">
+      <c r="Z47" s="72" t="s">
         <v>171</v>
       </c>
       <c r="AA47" s="14">
@@ -39350,7 +39366,7 @@
       <c r="Y48" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Z48" s="82" t="s">
+      <c r="Z48" s="72" t="s">
         <v>279</v>
       </c>
       <c r="AA48" s="14">
@@ -39398,7 +39414,7 @@
       <c r="R49" s="1"/>
       <c r="X49" s="60"/>
       <c r="Y49" s="5"/>
-      <c r="Z49" s="82"/>
+      <c r="Z49" s="72"/>
       <c r="AA49" s="14"/>
       <c r="AD49" s="17"/>
       <c r="AI49" s="68"/>
@@ -39432,7 +39448,7 @@
       <c r="R50" s="1"/>
       <c r="X50" s="60"/>
       <c r="Y50" s="5"/>
-      <c r="Z50" s="82"/>
+      <c r="Z50" s="72"/>
       <c r="AA50" s="14"/>
       <c r="AD50" s="17"/>
       <c r="AI50" s="68"/>
@@ -39466,7 +39482,7 @@
       <c r="R51" s="1"/>
       <c r="X51" s="60"/>
       <c r="Y51" s="5"/>
-      <c r="Z51" s="82"/>
+      <c r="Z51" s="72"/>
       <c r="AA51" s="14"/>
       <c r="AD51" s="17"/>
       <c r="AI51" s="68"/>
@@ -39537,7 +39553,7 @@
       <c r="Y52" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Z52" s="82" t="s">
+      <c r="Z52" s="72" t="s">
         <v>171</v>
       </c>
       <c r="AA52" s="14">
@@ -39652,53 +39668,53 @@
       </c>
     </row>
     <row r="58" spans="1:16369" s="63" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="79" t="s">
+      <c r="A58" s="80" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="79"/>
-      <c r="C58" s="79"/>
-      <c r="D58" s="79"/>
-      <c r="E58" s="79"/>
-      <c r="F58" s="79"/>
-      <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="79"/>
-      <c r="J58" s="79"/>
-      <c r="K58" s="79"/>
-      <c r="L58" s="79"/>
-      <c r="M58" s="79"/>
-      <c r="N58" s="79"/>
-      <c r="O58" s="79"/>
-      <c r="P58" s="79"/>
-      <c r="Q58" s="79"/>
-      <c r="R58" s="79"/>
-      <c r="S58" s="79"/>
-      <c r="T58" s="79"/>
-      <c r="U58" s="79"/>
-      <c r="V58" s="79"/>
-      <c r="W58" s="79"/>
-      <c r="X58" s="79"/>
-      <c r="Y58" s="79"/>
-      <c r="Z58" s="79"/>
-      <c r="AA58" s="79"/>
-      <c r="AB58" s="79"/>
-      <c r="AC58" s="79"/>
-      <c r="AD58" s="79"/>
-      <c r="AE58" s="79"/>
-      <c r="AF58" s="79"/>
-      <c r="AG58" s="79"/>
-      <c r="AH58" s="79"/>
-      <c r="AI58" s="79"/>
-      <c r="AJ58" s="79"/>
-      <c r="AK58" s="79"/>
-      <c r="AL58" s="79"/>
-      <c r="AM58" s="79"/>
-      <c r="AN58" s="79"/>
-      <c r="AO58" s="79"/>
-      <c r="AP58" s="79"/>
-      <c r="AQ58" s="79"/>
-      <c r="AR58" s="79"/>
-      <c r="AS58" s="79"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="80"/>
+      <c r="F58" s="80"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="80"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="80"/>
+      <c r="L58" s="80"/>
+      <c r="M58" s="80"/>
+      <c r="N58" s="80"/>
+      <c r="O58" s="80"/>
+      <c r="P58" s="80"/>
+      <c r="Q58" s="80"/>
+      <c r="R58" s="80"/>
+      <c r="S58" s="80"/>
+      <c r="T58" s="80"/>
+      <c r="U58" s="80"/>
+      <c r="V58" s="80"/>
+      <c r="W58" s="80"/>
+      <c r="X58" s="80"/>
+      <c r="Y58" s="80"/>
+      <c r="Z58" s="80"/>
+      <c r="AA58" s="80"/>
+      <c r="AB58" s="80"/>
+      <c r="AC58" s="80"/>
+      <c r="AD58" s="80"/>
+      <c r="AE58" s="80"/>
+      <c r="AF58" s="80"/>
+      <c r="AG58" s="80"/>
+      <c r="AH58" s="80"/>
+      <c r="AI58" s="80"/>
+      <c r="AJ58" s="80"/>
+      <c r="AK58" s="80"/>
+      <c r="AL58" s="80"/>
+      <c r="AM58" s="80"/>
+      <c r="AN58" s="80"/>
+      <c r="AO58" s="80"/>
+      <c r="AP58" s="80"/>
+      <c r="AQ58" s="80"/>
+      <c r="AR58" s="80"/>
+      <c r="AS58" s="80"/>
       <c r="AT58" s="64"/>
       <c r="AU58" s="64"/>
       <c r="AV58" s="64"/>
@@ -39763,55 +39779,55 @@
     </row>
     <row r="59" spans="1:16369" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
-      <c r="B59" s="73" t="s">
+      <c r="B59" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="C59" s="74"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="74"/>
-      <c r="J59" s="74"/>
-      <c r="K59" s="74"/>
-      <c r="L59" s="75"/>
-      <c r="M59" s="73" t="s">
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="83"/>
+      <c r="M59" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="N59" s="74"/>
-      <c r="O59" s="74"/>
-      <c r="P59" s="74"/>
-      <c r="Q59" s="74"/>
-      <c r="R59" s="75"/>
-      <c r="S59" s="73" t="s">
+      <c r="N59" s="82"/>
+      <c r="O59" s="82"/>
+      <c r="P59" s="82"/>
+      <c r="Q59" s="82"/>
+      <c r="R59" s="83"/>
+      <c r="S59" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="T59" s="74"/>
-      <c r="U59" s="74"/>
-      <c r="V59" s="74"/>
-      <c r="W59" s="74"/>
-      <c r="X59" s="75"/>
-      <c r="Y59" s="76" t="s">
+      <c r="T59" s="82"/>
+      <c r="U59" s="82"/>
+      <c r="V59" s="82"/>
+      <c r="W59" s="82"/>
+      <c r="X59" s="83"/>
+      <c r="Y59" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="Z59" s="77"/>
-      <c r="AA59" s="77"/>
-      <c r="AB59" s="77"/>
-      <c r="AC59" s="77"/>
-      <c r="AD59" s="78"/>
-      <c r="AE59" s="76" t="s">
+      <c r="Z59" s="84"/>
+      <c r="AA59" s="84"/>
+      <c r="AB59" s="84"/>
+      <c r="AC59" s="84"/>
+      <c r="AD59" s="76"/>
+      <c r="AE59" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="AF59" s="78"/>
-      <c r="AG59" s="76" t="s">
+      <c r="AF59" s="76"/>
+      <c r="AG59" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="AH59" s="78"/>
-      <c r="AI59" s="76" t="s">
+      <c r="AH59" s="76"/>
+      <c r="AI59" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="AJ59" s="78"/>
+      <c r="AJ59" s="76"/>
       <c r="AK59" s="18" t="s">
         <v>162</v>
       </c>
@@ -39821,14 +39837,14 @@
       <c r="AM59" s="20">
         <v>17.0626</v>
       </c>
-      <c r="AN59" s="70" t="s">
+      <c r="AN59" s="77" t="s">
         <v>163</v>
       </c>
-      <c r="AO59" s="71"/>
-      <c r="AP59" s="71"/>
-      <c r="AQ59" s="71"/>
-      <c r="AR59" s="71"/>
-      <c r="AS59" s="72"/>
+      <c r="AO59" s="78"/>
+      <c r="AP59" s="78"/>
+      <c r="AQ59" s="78"/>
+      <c r="AR59" s="78"/>
+      <c r="AS59" s="79"/>
       <c r="AT59" s="65"/>
       <c r="AU59" s="65"/>
       <c r="AV59" s="65"/>
@@ -72664,7 +72680,7 @@
       <c r="Y61" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z61" s="82" t="s">
+      <c r="Z61" s="72" t="s">
         <v>277</v>
       </c>
       <c r="AA61" s="14">
@@ -72737,7 +72753,7 @@
       <c r="Y62" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Z62" s="82" t="s">
+      <c r="Z62" s="72" t="s">
         <v>277</v>
       </c>
       <c r="AA62" s="14">
@@ -72765,6 +72781,14 @@
   </sheetData>
   <autoFilter ref="A2:AS62"/>
   <mergeCells count="17">
+    <mergeCell ref="AN1:AS1"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:X1"/>
+    <mergeCell ref="Y1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="AG59:AH59"/>
     <mergeCell ref="AI59:AJ59"/>
     <mergeCell ref="AN59:AS59"/>
@@ -72774,14 +72798,6 @@
     <mergeCell ref="S59:X59"/>
     <mergeCell ref="Y59:AD59"/>
     <mergeCell ref="AE59:AF59"/>
-    <mergeCell ref="AN1:AS1"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S1:X1"/>
-    <mergeCell ref="Y1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>